<commit_message>
Complete code. Fixed some errors and added new results to the results folder
</commit_message>
<xml_diff>
--- a/Some result data/Gene Set Enrichment results/Gene Set Enrichment - WikiPathways/GSEresultsWP_darkred_DCM_.xlsx
+++ b/Some result data/Gene Set Enrichment results/Gene Set Enrichment - WikiPathways/GSEresultsWP_darkred_DCM_.xlsx
@@ -168,16 +168,16 @@
         <v>-0.9230769230769231</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.66195563633704</v>
+        <v>-2.727932810637902</v>
       </c>
       <c r="F2" t="n">
-        <v>1.4870252989887154E-5</v>
+        <v>3.2516350321289134E-5</v>
       </c>
       <c r="G2" t="n">
-        <v>3.568860717572917E-4</v>
+        <v>7.803924077109392E-4</v>
       </c>
       <c r="H2" t="n">
-        <v>3.443637534500183E-4</v>
+        <v>7.530102179666957E-4</v>
       </c>
       <c r="I2" t="n">
         <v>11.0</v>
@@ -203,16 +203,16 @@
         <v>-0.68</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.23455331214101</v>
+        <v>-2.297730064065564</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0017863956508669251</v>
+        <v>0.0019006207657385234</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0214367478104031</v>
+        <v>0.02280744918886228</v>
       </c>
       <c r="H3" t="n">
-        <v>0.020684581220564397</v>
+        <v>0.022007187813814482</v>
       </c>
       <c r="I3" t="n">
         <v>25.0</v>

</xml_diff>